<commit_message>
Fix typo in farm frenzy 3
</commit_message>
<xml_diff>
--- a/Excel/farm_frenzy.xlsx
+++ b/Excel/farm_frenzy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD848644-9C3A-4408-9332-F0EDC10D8E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B900EE5E-1EEA-49A5-AF59-8E3FD2736857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -867,12 +867,6 @@
     <t>polished_pearls</t>
   </si>
   <si>
-    <t>Pearl Neklace</t>
-  </si>
-  <si>
-    <t>pearl_neklace</t>
-  </si>
-  <si>
     <t>Gold 2</t>
   </si>
   <si>
@@ -937,6 +931,12 @@
   </si>
   <si>
     <t>museum_ticket</t>
+  </si>
+  <si>
+    <t>Pearl Necklace</t>
+  </si>
+  <si>
+    <t>pearl_necklace</t>
   </si>
 </sst>
 </file>
@@ -2109,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6658F5F-E5F7-403D-BCBA-E39D3B76F158}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="B85" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="D85">
         <v>2000</v>
@@ -3061,10 +3061,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B86" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D86">
         <v>50</v>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B87" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D87">
         <v>2500</v>
@@ -3083,10 +3083,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B88" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D88">
         <v>2000</v>
@@ -3094,10 +3094,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B89" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D89">
         <v>10000</v>
@@ -3105,10 +3105,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B90" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D90">
         <v>20</v>
@@ -3116,10 +3116,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B91" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D91">
         <v>5000</v>
@@ -3127,10 +3127,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B92" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D92">
         <v>6000</v>
@@ -3138,10 +3138,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B93" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D93">
         <v>100</v>
@@ -3149,10 +3149,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B94" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D94">
         <v>8000</v>
@@ -3160,10 +3160,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B95" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D95">
         <v>1000</v>
@@ -3171,10 +3171,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B96" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D96">
         <v>15000</v>

</xml_diff>